<commit_message>
upload to s3 added
</commit_message>
<xml_diff>
--- a/json_urls/2022-11-23.xlsx
+++ b/json_urls/2022-11-23.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B442"/>
+  <dimension ref="A1:C445"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,6 +432,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71850461?host=hh.ru </t>
         </is>
       </c>
+      <c r="C1" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -444,6 +447,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/37640988?host=hh.ru </t>
         </is>
       </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -456,6 +462,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71573571?host=hh.ru </t>
         </is>
       </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -468,6 +477,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72775656?host=hh.ru </t>
         </is>
       </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -480,6 +492,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/47352925?host=hh.ru </t>
         </is>
       </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -492,6 +507,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70725259?host=hh.ru </t>
         </is>
       </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -504,6 +522,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72276632?host=hh.ru </t>
         </is>
       </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -516,6 +537,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/69893426?host=hh.ru </t>
         </is>
       </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -528,6 +552,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/68446916?host=hh.ru </t>
         </is>
       </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -540,6 +567,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71852829?host=hh.ru </t>
         </is>
       </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -552,6 +582,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/68947914?host=hh.ru </t>
         </is>
       </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -564,6 +597,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72043960?host=hh.ru </t>
         </is>
       </c>
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -576,6 +612,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66175026?host=hh.ru </t>
         </is>
       </c>
+      <c r="C13" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -588,6 +627,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72775658?host=hh.ru </t>
         </is>
       </c>
+      <c r="C14" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -600,6 +642,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/68702395?host=hh.ru </t>
         </is>
       </c>
+      <c r="C15" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -612,6 +657,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72276164?host=hh.ru </t>
         </is>
       </c>
+      <c r="C16" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -624,6 +672,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72775662?host=hh.ru </t>
         </is>
       </c>
+      <c r="C17" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -636,6 +687,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/53346652?host=hh.ru </t>
         </is>
       </c>
+      <c r="C18" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -648,6 +702,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/69329313?host=hh.ru </t>
         </is>
       </c>
+      <c r="C19" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -660,6 +717,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71645053?host=hh.ru </t>
         </is>
       </c>
+      <c r="C20" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -672,6 +732,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72276826?host=hh.ru </t>
         </is>
       </c>
+      <c r="C21" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -684,6 +747,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72774588?host=hh.ru </t>
         </is>
       </c>
+      <c r="C22" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -696,6 +762,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72045550?host=hh.ru </t>
         </is>
       </c>
+      <c r="C23" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -708,6 +777,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72337315?host=hh.ru </t>
         </is>
       </c>
+      <c r="C24" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -720,6 +792,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66175032?host=hh.ru </t>
         </is>
       </c>
+      <c r="C25" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -732,6 +807,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72045154?host=hh.ru </t>
         </is>
       </c>
+      <c r="C26" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -744,6 +822,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72200131?host=hh.ru </t>
         </is>
       </c>
+      <c r="C27" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -756,6 +837,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72199788?host=hh.ru </t>
         </is>
       </c>
+      <c r="C28" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -768,6 +852,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72774889?host=hh.ru </t>
         </is>
       </c>
+      <c r="C29" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -780,6 +867,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/68323684?host=hh.ru </t>
         </is>
       </c>
+      <c r="C30" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -792,6 +882,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71701823?host=hh.ru </t>
         </is>
       </c>
+      <c r="C31" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -804,6 +897,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/68860256?host=hh.ru </t>
         </is>
       </c>
+      <c r="C32" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -816,6 +912,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/69481610?host=hh.ru </t>
         </is>
       </c>
+      <c r="C33" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -828,6 +927,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71748221?host=hh.ru </t>
         </is>
       </c>
+      <c r="C34" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -840,6 +942,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/53557589?host=hh.ru </t>
         </is>
       </c>
+      <c r="C35" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -852,6 +957,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72277576?host=hh.ru </t>
         </is>
       </c>
+      <c r="C36" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -864,6 +972,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70846484?host=hh.ru </t>
         </is>
       </c>
+      <c r="C37" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -876,6 +987,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71486175?host=hh.ru </t>
         </is>
       </c>
+      <c r="C38" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -888,6 +1002,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72775865?host=hh.ru </t>
         </is>
       </c>
+      <c r="C39" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -900,6 +1017,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/68010452?host=hh.ru </t>
         </is>
       </c>
+      <c r="C40" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -912,6 +1032,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72476683?host=hh.ru </t>
         </is>
       </c>
+      <c r="C41" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -924,6 +1047,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71070488?host=hh.ru </t>
         </is>
       </c>
+      <c r="C42" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -936,6 +1062,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72276500?host=hh.ru </t>
         </is>
       </c>
+      <c r="C43" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -948,6 +1077,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70561390?host=hh.ru </t>
         </is>
       </c>
+      <c r="C44" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -960,6 +1092,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66506218?host=hh.ru </t>
         </is>
       </c>
+      <c r="C45" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -972,6 +1107,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/40882760?host=hh.ru </t>
         </is>
       </c>
+      <c r="C46" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -984,6 +1122,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70659530?host=hh.ru </t>
         </is>
       </c>
+      <c r="C47" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -996,6 +1137,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72443553?host=hh.ru </t>
         </is>
       </c>
+      <c r="C48" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1008,6 +1152,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70731819?host=hh.ru </t>
         </is>
       </c>
+      <c r="C49" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1020,6 +1167,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/68860257?host=hh.ru </t>
         </is>
       </c>
+      <c r="C50" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1032,6 +1182,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72775659?host=hh.ru </t>
         </is>
       </c>
+      <c r="C51" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1044,6 +1197,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70822329?host=hh.ru </t>
         </is>
       </c>
+      <c r="C52" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1056,6 +1212,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66863709?host=hh.ru </t>
         </is>
       </c>
+      <c r="C53" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1068,6 +1227,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72714545?host=hh.ru </t>
         </is>
       </c>
+      <c r="C54" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1080,6 +1242,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/67848766?host=hh.ru </t>
         </is>
       </c>
+      <c r="C55" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1092,6 +1257,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71322635?host=hh.ru </t>
         </is>
       </c>
+      <c r="C56" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1104,6 +1272,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/43981190?host=hh.ru </t>
         </is>
       </c>
+      <c r="C57" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1116,6 +1287,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71624737?host=hh.ru </t>
         </is>
       </c>
+      <c r="C58" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1128,6 +1302,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72276148?host=hh.ru </t>
         </is>
       </c>
+      <c r="C59" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1140,6 +1317,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71466782?host=hh.ru </t>
         </is>
       </c>
+      <c r="C60" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1152,6 +1332,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70974771?host=hh.ru </t>
         </is>
       </c>
+      <c r="C61" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1164,6 +1347,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72275871?host=hh.ru </t>
         </is>
       </c>
+      <c r="C62" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1176,6 +1362,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70324673?host=hh.ru </t>
         </is>
       </c>
+      <c r="C63" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1188,6 +1377,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72774728?host=hh.ru </t>
         </is>
       </c>
+      <c r="C64" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1200,6 +1392,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71431119?host=hh.ru </t>
         </is>
       </c>
+      <c r="C65" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1212,6 +1407,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72045475?host=hh.ru </t>
         </is>
       </c>
+      <c r="C66" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1224,6 +1422,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/69161868?host=hh.ru </t>
         </is>
       </c>
+      <c r="C67" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1236,6 +1437,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70654947?host=hh.ru </t>
         </is>
       </c>
+      <c r="C68" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1248,6 +1452,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71431254?host=hh.ru </t>
         </is>
       </c>
+      <c r="C69" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1260,6 +1467,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71512762?host=hh.ru </t>
         </is>
       </c>
+      <c r="C70" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1272,6 +1482,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/68929768?host=hh.ru </t>
         </is>
       </c>
+      <c r="C71" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1284,6 +1497,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72277350?host=hh.ru </t>
         </is>
       </c>
+      <c r="C72" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1296,6 +1512,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/69642393?host=hh.ru </t>
         </is>
       </c>
+      <c r="C73" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1308,6 +1527,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72444195?host=hh.ru </t>
         </is>
       </c>
+      <c r="C74" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1320,6 +1542,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71898213?host=hh.ru </t>
         </is>
       </c>
+      <c r="C75" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1332,6 +1557,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/68010464?host=hh.ru </t>
         </is>
       </c>
+      <c r="C76" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1344,6 +1572,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72045873?host=hh.ru </t>
         </is>
       </c>
+      <c r="C77" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1356,6 +1587,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71117890?host=hh.ru </t>
         </is>
       </c>
+      <c r="C78" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -1368,6 +1602,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/45437723?host=hh.ru </t>
         </is>
       </c>
+      <c r="C79" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1380,6 +1617,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71214395?host=hh.ru </t>
         </is>
       </c>
+      <c r="C80" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -1392,6 +1632,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72045511?host=hh.ru </t>
         </is>
       </c>
+      <c r="C81" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -1404,6 +1647,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70801588?host=hh.ru </t>
         </is>
       </c>
+      <c r="C82" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -1416,6 +1662,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/69123855?host=hh.ru </t>
         </is>
       </c>
+      <c r="C83" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -1428,6 +1677,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72769445?host=hh.ru </t>
         </is>
       </c>
+      <c r="C84" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -1440,6 +1692,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71959573?host=hh.ru </t>
         </is>
       </c>
+      <c r="C85" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -1452,6 +1707,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72769440?host=hh.ru </t>
         </is>
       </c>
+      <c r="C86" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -1464,6 +1722,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72438232?host=hh.ru </t>
         </is>
       </c>
+      <c r="C87" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -1476,6 +1737,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71641945?host=hh.ru </t>
         </is>
       </c>
+      <c r="C88" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -1488,6 +1752,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72196645?host=hh.ru </t>
         </is>
       </c>
+      <c r="C89" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -1500,6 +1767,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71987611?host=hh.ru </t>
         </is>
       </c>
+      <c r="C90" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -1512,6 +1782,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71642825?host=hh.ru </t>
         </is>
       </c>
+      <c r="C91" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -1524,6 +1797,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71987463?host=hh.ru </t>
         </is>
       </c>
+      <c r="C92" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -1536,6 +1812,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71588310?host=hh.ru </t>
         </is>
       </c>
+      <c r="C93" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -1548,6 +1827,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72769748?host=hh.ru </t>
         </is>
       </c>
+      <c r="C94" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -1560,6 +1842,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70779778?host=hh.ru </t>
         </is>
       </c>
+      <c r="C95" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -1572,6 +1857,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71748735?host=hh.ru </t>
         </is>
       </c>
+      <c r="C96" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -1584,6 +1872,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71534323?host=hh.ru </t>
         </is>
       </c>
+      <c r="C97" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -1596,6 +1887,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71465137?host=hh.ru </t>
         </is>
       </c>
+      <c r="C98" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -1608,6 +1902,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/67808106?host=hh.ru </t>
         </is>
       </c>
+      <c r="C99" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -1620,6 +1917,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71062160?host=hh.ru </t>
         </is>
       </c>
+      <c r="C100" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -1632,6 +1932,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71843722?host=hh.ru </t>
         </is>
       </c>
+      <c r="C101" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -1644,6 +1947,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72770069?host=hh.ru </t>
         </is>
       </c>
+      <c r="C102" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -1656,6 +1962,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72770188?host=hh.ru </t>
         </is>
       </c>
+      <c r="C103" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -1668,6 +1977,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72770067?host=hh.ru </t>
         </is>
       </c>
+      <c r="C104" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -1680,6 +1992,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72770066?host=hh.ru </t>
         </is>
       </c>
+      <c r="C105" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -1692,6 +2007,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72770068?host=hh.ru </t>
         </is>
       </c>
+      <c r="C106" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -1704,6 +2022,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72770184?host=hh.ru </t>
         </is>
       </c>
+      <c r="C107" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -1716,6 +2037,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/67053374?host=hh.ru </t>
         </is>
       </c>
+      <c r="C108" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -1728,6 +2052,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72770517?host=hh.ru </t>
         </is>
       </c>
+      <c r="C109" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -1740,6 +2067,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71290036?host=hh.ru </t>
         </is>
       </c>
+      <c r="C110" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -1752,6 +2082,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71599290?host=hh.ru </t>
         </is>
       </c>
+      <c r="C111" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -1764,6 +2097,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71843242?host=hh.ru </t>
         </is>
       </c>
+      <c r="C112" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -1776,6 +2112,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72770080?host=hh.ru </t>
         </is>
       </c>
+      <c r="C113" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -1788,6 +2127,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72769434?host=hh.ru </t>
         </is>
       </c>
+      <c r="C114" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -1800,6 +2142,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72770736?host=hh.ru </t>
         </is>
       </c>
+      <c r="C115" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -1812,6 +2157,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71959136?host=hh.ru </t>
         </is>
       </c>
+      <c r="C116" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -1824,6 +2172,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70555201?host=hh.ru </t>
         </is>
       </c>
+      <c r="C117" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -1836,6 +2187,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72769112?host=hh.ru </t>
         </is>
       </c>
+      <c r="C118" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -1848,6 +2202,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/68131257?host=hh.ru </t>
         </is>
       </c>
+      <c r="C119" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -1860,6 +2217,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72270616?host=hh.ru </t>
         </is>
       </c>
+      <c r="C120" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -1872,6 +2232,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72770514?host=hh.ru </t>
         </is>
       </c>
+      <c r="C121" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -1884,6 +2247,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71128349?host=hh.ru </t>
         </is>
       </c>
+      <c r="C122" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -1896,6 +2262,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72040441?host=hh.ru </t>
         </is>
       </c>
+      <c r="C123" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -1908,6 +2277,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70470936?host=hh.ru </t>
         </is>
       </c>
+      <c r="C124" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -1920,6 +2292,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72770404?host=hh.ru </t>
         </is>
       </c>
+      <c r="C125" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -1932,6 +2307,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71641797?host=hh.ru </t>
         </is>
       </c>
+      <c r="C126" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -1944,6 +2322,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72770070?host=hh.ru </t>
         </is>
       </c>
+      <c r="C127" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -1956,6 +2337,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71533937?host=hh.ru </t>
         </is>
       </c>
+      <c r="C128" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -1968,6 +2352,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72770065?host=hh.ru </t>
         </is>
       </c>
+      <c r="C129" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -1980,6 +2367,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/69279779?host=hh.ru </t>
         </is>
       </c>
+      <c r="C130" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -1992,6 +2382,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70668877?host=hh.ru </t>
         </is>
       </c>
+      <c r="C131" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -2004,6 +2397,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71573190?host=hh.ru </t>
         </is>
       </c>
+      <c r="C132" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -2016,6 +2412,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72196667?host=hh.ru </t>
         </is>
       </c>
+      <c r="C133" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -2028,6 +2427,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/69010850?host=hh.ru </t>
         </is>
       </c>
+      <c r="C134" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -2040,6 +2442,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70324238?host=hh.ru </t>
         </is>
       </c>
+      <c r="C135" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -2052,6 +2457,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70499027?host=hh.ru </t>
         </is>
       </c>
+      <c r="C136" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -2064,6 +2472,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70441534?host=hh.ru </t>
         </is>
       </c>
+      <c r="C137" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -2076,6 +2487,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72040379?host=hh.ru </t>
         </is>
       </c>
+      <c r="C138" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -2088,6 +2502,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72039322?host=hh.ru </t>
         </is>
       </c>
+      <c r="C139" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -2100,6 +2517,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70499028?host=hh.ru </t>
         </is>
       </c>
+      <c r="C140" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -2112,6 +2532,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71686659?host=hh.ru </t>
         </is>
       </c>
+      <c r="C141" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -2124,6 +2547,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/69737647?host=hh.ru </t>
         </is>
       </c>
+      <c r="C142" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -2136,6 +2562,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71092137?host=hh.ru </t>
         </is>
       </c>
+      <c r="C143" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -2148,6 +2577,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72040418?host=hh.ru </t>
         </is>
       </c>
+      <c r="C144" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -2160,6 +2592,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71521355?host=hh.ru </t>
         </is>
       </c>
+      <c r="C145" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -2172,6 +2607,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/54833451?host=hh.ru </t>
         </is>
       </c>
+      <c r="C146" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -2184,6 +2622,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71289724?host=hh.ru </t>
         </is>
       </c>
+      <c r="C147" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -2196,6 +2637,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/69737592?host=hh.ru </t>
         </is>
       </c>
+      <c r="C148" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -2208,6 +2652,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/67598895?host=hh.ru </t>
         </is>
       </c>
+      <c r="C149" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -2220,6 +2667,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71959122?host=hh.ru </t>
         </is>
       </c>
+      <c r="C150" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -2232,6 +2682,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72768787?host=hh.ru </t>
         </is>
       </c>
+      <c r="C151" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -2244,6 +2697,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72768474?host=hh.ru </t>
         </is>
       </c>
+      <c r="C152" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -2256,6 +2712,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72768469?host=hh.ru </t>
         </is>
       </c>
+      <c r="C153" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -2268,6 +2727,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72693744?host=hh.ru </t>
         </is>
       </c>
+      <c r="C154" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -2280,6 +2742,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72195490?host=hh.ru </t>
         </is>
       </c>
+      <c r="C155" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -2292,6 +2757,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72768788?host=hh.ru </t>
         </is>
       </c>
+      <c r="C156" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -2304,6 +2772,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72768785?host=hh.ru </t>
         </is>
       </c>
+      <c r="C157" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -2316,6 +2787,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71504983?host=hh.ru </t>
         </is>
       </c>
+      <c r="C158" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -2328,6 +2802,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72768606?host=hh.ru </t>
         </is>
       </c>
+      <c r="C159" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -2340,6 +2817,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72768605?host=hh.ru </t>
         </is>
       </c>
+      <c r="C160" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -2352,6 +2832,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72768492?host=hh.ru </t>
         </is>
       </c>
+      <c r="C161" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -2364,6 +2847,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71490998?host=hh.ru </t>
         </is>
       </c>
+      <c r="C162" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -2376,6 +2862,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71489929?host=hh.ru </t>
         </is>
       </c>
+      <c r="C163" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -2388,6 +2877,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71565240?host=hh.ru </t>
         </is>
       </c>
+      <c r="C164" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -2400,6 +2892,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72768495?host=hh.ru </t>
         </is>
       </c>
+      <c r="C165" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -2412,6 +2907,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72302618?host=hh.ru </t>
         </is>
       </c>
+      <c r="C166" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -2424,6 +2922,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72768473?host=hh.ru </t>
         </is>
       </c>
+      <c r="C167" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -2436,6 +2937,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71081379?host=hh.ru </t>
         </is>
       </c>
+      <c r="C168" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -2448,6 +2952,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70860653?host=hh.ru </t>
         </is>
       </c>
+      <c r="C169" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -2460,6 +2967,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72768599?host=hh.ru </t>
         </is>
       </c>
+      <c r="C170" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -2472,6 +2982,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71413970?host=hh.ru </t>
         </is>
       </c>
+      <c r="C171" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -2484,6 +2997,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72683546?host=hh.ru </t>
         </is>
       </c>
+      <c r="C172" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -2496,6 +3012,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71492030?host=hh.ru </t>
         </is>
       </c>
+      <c r="C173" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -2508,6 +3027,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71815234?host=hh.ru </t>
         </is>
       </c>
+      <c r="C174" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -2520,6 +3042,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71723190?host=hh.ru </t>
         </is>
       </c>
+      <c r="C175" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -2532,6 +3057,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71625648?host=hh.ru </t>
         </is>
       </c>
+      <c r="C176" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -2544,6 +3072,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71635568?host=hh.ru </t>
         </is>
       </c>
+      <c r="C177" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -2556,6 +3087,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72184351?host=hh.ru </t>
         </is>
       </c>
+      <c r="C178" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -2568,6 +3102,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72195800?host=hh.ru </t>
         </is>
       </c>
+      <c r="C179" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -2580,6 +3117,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/54470306?host=hh.ru </t>
         </is>
       </c>
+      <c r="C180" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -2592,6 +3132,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72436736?host=hh.ru </t>
         </is>
       </c>
+      <c r="C181" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -2604,6 +3147,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70349647?host=hh.ru </t>
         </is>
       </c>
+      <c r="C182" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -2616,6 +3162,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71641729?host=hh.ru </t>
         </is>
       </c>
+      <c r="C183" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -2628,6 +3177,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71641712?host=hh.ru </t>
         </is>
       </c>
+      <c r="C184" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -2640,6 +3192,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72490319?host=hh.ru </t>
         </is>
       </c>
+      <c r="C185" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -2652,6 +3207,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/49032849?host=hh.ru </t>
         </is>
       </c>
+      <c r="C186" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -2664,6 +3222,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70462828?host=hh.ru </t>
         </is>
       </c>
+      <c r="C187" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -2676,6 +3237,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71870557?host=hh.ru </t>
         </is>
       </c>
+      <c r="C188" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -2688,6 +3252,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72796400?host=hh.ru </t>
         </is>
       </c>
+      <c r="C189" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -2700,6 +3267,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71071166?host=hh.ru </t>
         </is>
       </c>
+      <c r="C190" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -2712,6 +3282,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/42949326?host=hh.ru </t>
         </is>
       </c>
+      <c r="C191" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -2724,6 +3297,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72464341?host=hh.ru </t>
         </is>
       </c>
+      <c r="C192" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -2736,6 +3312,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71868136?host=hh.ru </t>
         </is>
       </c>
+      <c r="C193" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -2748,6 +3327,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72463062?host=hh.ru </t>
         </is>
       </c>
+      <c r="C194" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -2760,6 +3342,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72228799?host=hh.ru </t>
         </is>
       </c>
+      <c r="C195" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -2772,6 +3357,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71679873?host=hh.ru </t>
         </is>
       </c>
+      <c r="C196" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -2784,6 +3372,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71938687?host=hh.ru </t>
         </is>
       </c>
+      <c r="C197" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -2796,6 +3387,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70886238?host=hh.ru </t>
         </is>
       </c>
+      <c r="C198" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -2808,6 +3402,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70676818?host=hh.ru </t>
         </is>
       </c>
+      <c r="C199" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -2820,6 +3417,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72018976?host=hh.ru </t>
         </is>
       </c>
+      <c r="C200" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -2832,6 +3432,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72066369?host=hh.ru </t>
         </is>
       </c>
+      <c r="C201" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -2844,6 +3447,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72296073?host=hh.ru </t>
         </is>
       </c>
+      <c r="C202" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -2856,6 +3462,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72216270?host=hh.ru </t>
         </is>
       </c>
+      <c r="C203" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -2868,6 +3477,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/69314710?host=hh.ru </t>
         </is>
       </c>
+      <c r="C204" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -2880,6 +3492,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72216040?host=hh.ru </t>
         </is>
       </c>
+      <c r="C205" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -2892,6 +3507,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/69258305?host=hh.ru </t>
         </is>
       </c>
+      <c r="C206" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -2904,6 +3522,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71409704?host=hh.ru </t>
         </is>
       </c>
+      <c r="C207" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -2916,6 +3537,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860020?host=hh.ru </t>
         </is>
       </c>
+      <c r="C208" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -2928,6 +3552,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/68830766?host=hh.ru </t>
         </is>
       </c>
+      <c r="C209" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -2940,6 +3567,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71103343?host=hh.ru </t>
         </is>
       </c>
+      <c r="C210" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -2952,6 +3582,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71662510?host=hh.ru </t>
         </is>
       </c>
+      <c r="C211" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -2964,6 +3597,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72297437?host=hh.ru </t>
         </is>
       </c>
+      <c r="C212" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -2976,6 +3612,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71867799?host=hh.ru </t>
         </is>
       </c>
+      <c r="C213" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -2988,6 +3627,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72296151?host=hh.ru </t>
         </is>
       </c>
+      <c r="C214" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -3000,6 +3642,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/48275276?host=hh.ru </t>
         </is>
       </c>
+      <c r="C215" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -3012,6 +3657,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71658860?host=hh.ru </t>
         </is>
       </c>
+      <c r="C216" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -3024,6 +3672,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71659690?host=hh.ru </t>
         </is>
       </c>
+      <c r="C217" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -3036,6 +3687,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72795468?host=hh.ru </t>
         </is>
       </c>
+      <c r="C218" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -3048,6 +3702,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71659166?host=hh.ru </t>
         </is>
       </c>
+      <c r="C219" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -3060,6 +3717,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71867797?host=hh.ru </t>
         </is>
       </c>
+      <c r="C220" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -3072,6 +3732,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/67489738?host=hh.ru </t>
         </is>
       </c>
+      <c r="C221" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -3084,6 +3747,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71409664?host=hh.ru </t>
         </is>
       </c>
+      <c r="C222" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -3096,6 +3762,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72121440?host=hh.ru </t>
         </is>
       </c>
+      <c r="C223" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -3108,6 +3777,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72299961?host=hh.ru </t>
         </is>
       </c>
+      <c r="C224" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -3120,6 +3792,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860532?host=hh.ru </t>
         </is>
       </c>
+      <c r="C225" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -3132,6 +3807,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72793510?host=hh.ru </t>
         </is>
       </c>
+      <c r="C226" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -3144,6 +3822,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71660383?host=hh.ru </t>
         </is>
       </c>
+      <c r="C227" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -3156,6 +3837,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71602450?host=hh.ru </t>
         </is>
       </c>
+      <c r="C228" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -3168,6 +3852,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72794568?host=hh.ru </t>
         </is>
       </c>
+      <c r="C229" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -3180,6 +3867,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71212843?host=hh.ru </t>
         </is>
       </c>
+      <c r="C230" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -3192,6 +3882,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860235?host=hh.ru </t>
         </is>
       </c>
+      <c r="C231" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -3204,6 +3897,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860157?host=hh.ru </t>
         </is>
       </c>
+      <c r="C232" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -3216,6 +3912,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70459119?host=hh.ru </t>
         </is>
       </c>
+      <c r="C233" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -3228,6 +3927,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72463036?host=hh.ru </t>
         </is>
       </c>
+      <c r="C234" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -3240,6 +3942,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70017478?host=hh.ru </t>
         </is>
       </c>
+      <c r="C235" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -3252,6 +3957,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71662581?host=hh.ru </t>
         </is>
       </c>
+      <c r="C236" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -3264,6 +3972,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72072922?host=hh.ru </t>
         </is>
       </c>
+      <c r="C237" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -3276,6 +3987,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/69252938?host=hh.ru </t>
         </is>
       </c>
+      <c r="C238" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -3288,6 +4002,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72297673?host=hh.ru </t>
         </is>
       </c>
+      <c r="C239" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -3300,6 +4017,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71662276?host=hh.ru </t>
         </is>
       </c>
+      <c r="C240" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -3312,6 +4032,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70407757?host=hh.ru </t>
         </is>
       </c>
+      <c r="C241" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -3324,6 +4047,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/42961353?host=hh.ru </t>
         </is>
       </c>
+      <c r="C242" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -3336,6 +4062,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71868263?host=hh.ru </t>
         </is>
       </c>
+      <c r="C243" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -3348,6 +4077,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71259663?host=hh.ru </t>
         </is>
       </c>
+      <c r="C244" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -3360,6 +4092,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71806347?host=hh.ru </t>
         </is>
       </c>
+      <c r="C245" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -3372,6 +4107,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72217253?host=hh.ru </t>
         </is>
       </c>
+      <c r="C246" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -3384,6 +4122,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71494879?host=hh.ru </t>
         </is>
       </c>
+      <c r="C247" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -3396,6 +4137,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72064471?host=hh.ru </t>
         </is>
       </c>
+      <c r="C248" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -3408,6 +4152,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/68947618?host=hh.ru </t>
         </is>
       </c>
+      <c r="C249" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -3420,6 +4167,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71662186?host=hh.ru </t>
         </is>
       </c>
+      <c r="C250" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -3432,6 +4182,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72541940?host=hh.ru </t>
         </is>
       </c>
+      <c r="C251" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -3444,6 +4197,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/67640111?host=hh.ru </t>
         </is>
       </c>
+      <c r="C252" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -3456,6 +4212,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72229581?host=hh.ru </t>
         </is>
       </c>
+      <c r="C253" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -3468,6 +4227,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/51099502?host=hh.ru </t>
         </is>
       </c>
+      <c r="C254" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -3480,6 +4242,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71661934?host=hh.ru </t>
         </is>
       </c>
+      <c r="C255" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -3492,6 +4257,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71662727?host=hh.ru </t>
         </is>
       </c>
+      <c r="C256" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -3504,6 +4272,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/54134941?host=hh.ru </t>
         </is>
       </c>
+      <c r="C257" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -3516,6 +4287,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70575343?host=hh.ru </t>
         </is>
       </c>
+      <c r="C258" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -3528,6 +4302,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71107712?host=hh.ru </t>
         </is>
       </c>
+      <c r="C259" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -3540,6 +4317,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/68648182?host=hh.ru </t>
         </is>
       </c>
+      <c r="C260" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -3552,6 +4332,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71506510?host=hh.ru </t>
         </is>
       </c>
+      <c r="C261" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -3564,6 +4347,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72065377?host=hh.ru </t>
         </is>
       </c>
+      <c r="C262" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -3576,6 +4362,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72216601?host=hh.ru </t>
         </is>
       </c>
+      <c r="C263" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -3588,6 +4377,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72066257?host=hh.ru </t>
         </is>
       </c>
+      <c r="C264" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
@@ -3600,6 +4392,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71660602?host=hh.ru </t>
         </is>
       </c>
+      <c r="C265" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
@@ -3612,6 +4407,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71494880?host=hh.ru </t>
         </is>
       </c>
+      <c r="C266" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
@@ -3624,6 +4422,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70337158?host=hh.ru </t>
         </is>
       </c>
+      <c r="C267" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -3636,6 +4437,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70685359?host=hh.ru </t>
         </is>
       </c>
+      <c r="C268" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -3648,6 +4452,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72296283?host=hh.ru </t>
         </is>
       </c>
+      <c r="C269" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -3660,6 +4467,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70725022?host=hh.ru </t>
         </is>
       </c>
+      <c r="C270" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
@@ -3672,6 +4482,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71695467?host=hh.ru </t>
         </is>
       </c>
+      <c r="C271" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
@@ -3684,6 +4497,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/67448661?host=hh.ru </t>
         </is>
       </c>
+      <c r="C272" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
@@ -3696,6 +4512,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72215133?host=hh.ru </t>
         </is>
       </c>
+      <c r="C273" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
@@ -3708,6 +4527,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72063782?host=hh.ru </t>
         </is>
       </c>
+      <c r="C274" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -3720,6 +4542,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70405056?host=hh.ru </t>
         </is>
       </c>
+      <c r="C275" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -3732,6 +4557,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72465310?host=hh.ru </t>
         </is>
       </c>
+      <c r="C276" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -3744,6 +4572,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/69864626?host=hh.ru </t>
         </is>
       </c>
+      <c r="C277" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
@@ -3756,6 +4587,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72296209?host=hh.ru </t>
         </is>
       </c>
+      <c r="C278" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -3768,6 +4602,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72792307?host=hh.ru </t>
         </is>
       </c>
+      <c r="C279" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -3780,6 +4617,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71655782?host=hh.ru </t>
         </is>
       </c>
+      <c r="C280" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -3792,6 +4632,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72123911?host=hh.ru </t>
         </is>
       </c>
+      <c r="C281" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -3804,6 +4647,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71274106?host=hh.ru </t>
         </is>
       </c>
+      <c r="C282" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
@@ -3816,6 +4662,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71868231?host=hh.ru </t>
         </is>
       </c>
+      <c r="C283" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
@@ -3828,6 +4677,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66221926?host=hh.ru </t>
         </is>
       </c>
+      <c r="C284" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
@@ -3840,6 +4692,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71519407?host=hh.ru </t>
         </is>
       </c>
+      <c r="C285" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
@@ -3852,6 +4707,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70677213?host=hh.ru </t>
         </is>
       </c>
+      <c r="C286" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
@@ -3864,6 +4722,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71870527?host=hh.ru </t>
         </is>
       </c>
+      <c r="C287" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
@@ -3876,6 +4737,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/67363462?host=hh.ru </t>
         </is>
       </c>
+      <c r="C288" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
@@ -3888,6 +4752,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71049822?host=hh.ru </t>
         </is>
       </c>
+      <c r="C289" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
@@ -3900,6 +4767,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72297998?host=hh.ru </t>
         </is>
       </c>
+      <c r="C290" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
@@ -3912,6 +4782,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71868439?host=hh.ru </t>
         </is>
       </c>
+      <c r="C291" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
@@ -3924,6 +4797,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72793487?host=hh.ru </t>
         </is>
       </c>
+      <c r="C292" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
@@ -3936,6 +4812,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72217741?host=hh.ru </t>
         </is>
       </c>
+      <c r="C293" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
@@ -3948,6 +4827,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71866350?host=hh.ru </t>
         </is>
       </c>
+      <c r="C294" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
@@ -3960,6 +4842,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/67448170?host=hh.ru </t>
         </is>
       </c>
+      <c r="C295" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
@@ -3972,6 +4857,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72066236?host=hh.ru </t>
         </is>
       </c>
+      <c r="C296" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
@@ -3984,6 +4872,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72796038?host=hh.ru </t>
         </is>
       </c>
+      <c r="C297" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
@@ -3996,6 +4887,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860388?host=hh.ru </t>
         </is>
       </c>
+      <c r="C298" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
@@ -4008,6 +4902,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71263834?host=hh.ru </t>
         </is>
       </c>
+      <c r="C299" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
@@ -4020,6 +4917,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72297127?host=hh.ru </t>
         </is>
       </c>
+      <c r="C300" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
@@ -4032,6 +4932,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/69166503?host=hh.ru </t>
         </is>
       </c>
+      <c r="C301" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
@@ -4044,6 +4947,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72169417?host=hh.ru </t>
         </is>
       </c>
+      <c r="C302" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
@@ -4056,6 +4962,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72206138?host=hh.ru </t>
         </is>
       </c>
+      <c r="C303" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
@@ -4068,6 +4977,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860301?host=hh.ru </t>
         </is>
       </c>
+      <c r="C304" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
@@ -4080,6 +4992,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72300527?host=hh.ru </t>
         </is>
       </c>
+      <c r="C305" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
@@ -4092,6 +5007,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72065106?host=hh.ru </t>
         </is>
       </c>
+      <c r="C306" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
@@ -4104,6 +5022,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70371606?host=hh.ru </t>
         </is>
       </c>
+      <c r="C307" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
@@ -4116,6 +5037,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71661614?host=hh.ru </t>
         </is>
       </c>
+      <c r="C308" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
@@ -4128,6 +5052,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71660577?host=hh.ru </t>
         </is>
       </c>
+      <c r="C309" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
@@ -4140,6 +5067,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72216787?host=hh.ru </t>
         </is>
       </c>
+      <c r="C310" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
@@ -4152,6 +5082,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72299765?host=hh.ru </t>
         </is>
       </c>
+      <c r="C311" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
@@ -4164,6 +5097,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72464771?host=hh.ru </t>
         </is>
       </c>
+      <c r="C312" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
@@ -4176,6 +5112,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71869304?host=hh.ru </t>
         </is>
       </c>
+      <c r="C313" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
@@ -4188,6 +5127,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72215520?host=hh.ru </t>
         </is>
       </c>
+      <c r="C314" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
@@ -4200,6 +5142,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71869455?host=hh.ru </t>
         </is>
       </c>
+      <c r="C315" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
@@ -4212,6 +5157,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72332994?host=hh.ru </t>
         </is>
       </c>
+      <c r="C316" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
@@ -4224,6 +5172,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72426326?host=hh.ru </t>
         </is>
       </c>
+      <c r="C317" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
@@ -4236,6 +5187,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/51270006?host=hh.ru </t>
         </is>
       </c>
+      <c r="C318" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
@@ -4248,6 +5202,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71761668?host=hh.ru </t>
         </is>
       </c>
+      <c r="C319" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
@@ -4260,6 +5217,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860553?host=hh.ru </t>
         </is>
       </c>
+      <c r="C320" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
@@ -4272,6 +5232,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72793257?host=hh.ru </t>
         </is>
       </c>
+      <c r="C321" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
@@ -4284,6 +5247,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72297454?host=hh.ru </t>
         </is>
       </c>
+      <c r="C322" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
@@ -4296,6 +5262,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71595474?host=hh.ru </t>
         </is>
       </c>
+      <c r="C323" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
@@ -4308,6 +5277,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71867794?host=hh.ru </t>
         </is>
       </c>
+      <c r="C324" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
@@ -4320,6 +5292,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860026?host=hh.ru </t>
         </is>
       </c>
+      <c r="C325" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
@@ -4332,6 +5307,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71870518?host=hh.ru </t>
         </is>
       </c>
+      <c r="C326" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
@@ -4344,6 +5322,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72067454?host=hh.ru </t>
         </is>
       </c>
+      <c r="C327" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
@@ -4356,6 +5337,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72065196?host=hh.ru </t>
         </is>
       </c>
+      <c r="C328" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
@@ -4368,6 +5352,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72064811?host=hh.ru </t>
         </is>
       </c>
+      <c r="C329" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
@@ -4380,6 +5367,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71556091?host=hh.ru </t>
         </is>
       </c>
+      <c r="C330" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
@@ -4392,6 +5382,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72217061?host=hh.ru </t>
         </is>
       </c>
+      <c r="C331" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
@@ -4404,6 +5397,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66859858?host=hh.ru </t>
         </is>
       </c>
+      <c r="C332" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
@@ -4416,6 +5412,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860188?host=hh.ru </t>
         </is>
       </c>
+      <c r="C333" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
@@ -4428,6 +5427,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71659063?host=hh.ru </t>
         </is>
       </c>
+      <c r="C334" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
@@ -4440,6 +5442,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72065080?host=hh.ru </t>
         </is>
       </c>
+      <c r="C335" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
@@ -4452,6 +5457,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72066216?host=hh.ru </t>
         </is>
       </c>
+      <c r="C336" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
@@ -4464,6 +5472,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/67571815?host=hh.ru </t>
         </is>
       </c>
+      <c r="C337" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
@@ -4476,6 +5487,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72217657?host=hh.ru </t>
         </is>
       </c>
+      <c r="C338" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
@@ -4488,6 +5502,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72064863?host=hh.ru </t>
         </is>
       </c>
+      <c r="C339" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
@@ -4500,6 +5517,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72215563?host=hh.ru </t>
         </is>
       </c>
+      <c r="C340" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
@@ -4512,6 +5532,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72793931?host=hh.ru </t>
         </is>
       </c>
+      <c r="C341" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
@@ -4524,6 +5547,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860527?host=hh.ru </t>
         </is>
       </c>
+      <c r="C342" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
@@ -4536,6 +5562,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860319?host=hh.ru </t>
         </is>
       </c>
+      <c r="C343" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
@@ -4548,6 +5577,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71660360?host=hh.ru </t>
         </is>
       </c>
+      <c r="C344" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
@@ -4560,6 +5592,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72065008?host=hh.ru </t>
         </is>
       </c>
+      <c r="C345" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
@@ -4572,6 +5607,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72067192?host=hh.ru </t>
         </is>
       </c>
+      <c r="C346" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
@@ -4584,6 +5622,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/55028606?host=hh.ru </t>
         </is>
       </c>
+      <c r="C347" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
@@ -4596,6 +5637,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/69165261?host=hh.ru </t>
         </is>
       </c>
+      <c r="C348" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
@@ -4608,6 +5652,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71136017?host=hh.ru </t>
         </is>
       </c>
+      <c r="C349" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
@@ -4620,6 +5667,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72793483?host=hh.ru </t>
         </is>
       </c>
+      <c r="C350" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
@@ -4632,6 +5682,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66859888?host=hh.ru </t>
         </is>
       </c>
+      <c r="C351" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
@@ -4644,6 +5697,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860579?host=hh.ru </t>
         </is>
       </c>
+      <c r="C352" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
@@ -4656,6 +5712,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860213?host=hh.ru </t>
         </is>
       </c>
+      <c r="C353" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
@@ -4668,6 +5727,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72465827?host=hh.ru </t>
         </is>
       </c>
+      <c r="C354" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
@@ -4680,6 +5742,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860278?host=hh.ru </t>
         </is>
       </c>
+      <c r="C355" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
@@ -4692,6 +5757,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72792164?host=hh.ru </t>
         </is>
       </c>
+      <c r="C356" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
@@ -4704,6 +5772,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71042618?host=hh.ru </t>
         </is>
       </c>
+      <c r="C357" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
@@ -4716,6 +5787,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860516?host=hh.ru </t>
         </is>
       </c>
+      <c r="C358" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
@@ -4728,6 +5802,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860372?host=hh.ru </t>
         </is>
       </c>
+      <c r="C359" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
@@ -4740,6 +5817,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71641186?host=hh.ru </t>
         </is>
       </c>
+      <c r="C360" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
@@ -4752,6 +5832,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71870044?host=hh.ru </t>
         </is>
       </c>
+      <c r="C361" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
@@ -4764,6 +5847,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72793960?host=hh.ru </t>
         </is>
       </c>
+      <c r="C362" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
@@ -4776,6 +5862,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71659386?host=hh.ru </t>
         </is>
       </c>
+      <c r="C363" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
@@ -4788,6 +5877,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860268?host=hh.ru </t>
         </is>
       </c>
+      <c r="C364" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
@@ -4800,6 +5892,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72216026?host=hh.ru </t>
         </is>
       </c>
+      <c r="C365" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
@@ -4812,6 +5907,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860179?host=hh.ru </t>
         </is>
       </c>
+      <c r="C366" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
@@ -4824,6 +5922,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71488348?host=hh.ru </t>
         </is>
       </c>
+      <c r="C367" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
@@ -4836,6 +5937,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/67365638?host=hh.ru </t>
         </is>
       </c>
+      <c r="C368" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
@@ -4848,6 +5952,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66859951?host=hh.ru </t>
         </is>
       </c>
+      <c r="C369" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
@@ -4860,6 +5967,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860010?host=hh.ru </t>
         </is>
       </c>
+      <c r="C370" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
@@ -4872,6 +5982,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860489?host=hh.ru </t>
         </is>
       </c>
+      <c r="C371" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
@@ -4884,6 +5997,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860225?host=hh.ru </t>
         </is>
       </c>
+      <c r="C372" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
@@ -4896,6 +6012,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72793930?host=hh.ru </t>
         </is>
       </c>
+      <c r="C373" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
@@ -4908,6 +6027,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72793484?host=hh.ru </t>
         </is>
       </c>
+      <c r="C374" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
@@ -4920,6 +6042,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72793905?host=hh.ru </t>
         </is>
       </c>
+      <c r="C375" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
@@ -4932,6 +6057,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72297222?host=hh.ru </t>
         </is>
       </c>
+      <c r="C376" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
@@ -4944,6 +6072,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/54368183?host=hh.ru </t>
         </is>
       </c>
+      <c r="C377" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
@@ -4956,6 +6087,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72462195?host=hh.ru </t>
         </is>
       </c>
+      <c r="C378" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
@@ -4968,6 +6102,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72215703?host=hh.ru </t>
         </is>
       </c>
+      <c r="C379" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
@@ -4980,6 +6117,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71655104?host=hh.ru </t>
         </is>
       </c>
+      <c r="C380" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
@@ -4992,6 +6132,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72795575?host=hh.ru </t>
         </is>
       </c>
+      <c r="C381" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
@@ -5004,6 +6147,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860560?host=hh.ru </t>
         </is>
       </c>
+      <c r="C382" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
@@ -5016,6 +6162,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66859882?host=hh.ru </t>
         </is>
       </c>
+      <c r="C383" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
@@ -5028,6 +6177,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72064654?host=hh.ru </t>
         </is>
       </c>
+      <c r="C384" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="385">
       <c r="A385" t="inlineStr">
@@ -5040,6 +6192,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860259?host=hh.ru </t>
         </is>
       </c>
+      <c r="C385" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
@@ -5052,6 +6207,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/54367367?host=hh.ru </t>
         </is>
       </c>
+      <c r="C386" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">
@@ -5064,6 +6222,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860566?host=hh.ru </t>
         </is>
       </c>
+      <c r="C387" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="388">
       <c r="A388" t="inlineStr">
@@ -5076,6 +6237,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72064612?host=hh.ru </t>
         </is>
       </c>
+      <c r="C388" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="389">
       <c r="A389" t="inlineStr">
@@ -5088,6 +6252,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72066404?host=hh.ru </t>
         </is>
       </c>
+      <c r="C389" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="390">
       <c r="A390" t="inlineStr">
@@ -5100,6 +6267,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860147?host=hh.ru </t>
         </is>
       </c>
+      <c r="C390" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="391">
       <c r="A391" t="inlineStr">
@@ -5112,6 +6282,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72065139?host=hh.ru </t>
         </is>
       </c>
+      <c r="C391" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="392">
       <c r="A392" t="inlineStr">
@@ -5124,6 +6297,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860336?host=hh.ru </t>
         </is>
       </c>
+      <c r="C392" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="393">
       <c r="A393" t="inlineStr">
@@ -5136,6 +6312,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72064945?host=hh.ru </t>
         </is>
       </c>
+      <c r="C393" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="394">
       <c r="A394" t="inlineStr">
@@ -5148,6 +6327,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72066316?host=hh.ru </t>
         </is>
       </c>
+      <c r="C394" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="395">
       <c r="A395" t="inlineStr">
@@ -5160,6 +6342,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72510903?host=hh.ru </t>
         </is>
       </c>
+      <c r="C395" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="396">
       <c r="A396" t="inlineStr">
@@ -5172,6 +6357,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72794013?host=hh.ru </t>
         </is>
       </c>
+      <c r="C396" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="397">
       <c r="A397" t="inlineStr">
@@ -5184,6 +6372,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/69988113?host=hh.ru </t>
         </is>
       </c>
+      <c r="C397" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="398">
       <c r="A398" t="inlineStr">
@@ -5196,6 +6387,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860591?host=hh.ru </t>
         </is>
       </c>
+      <c r="C398" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="399">
       <c r="A399" t="inlineStr">
@@ -5208,6 +6402,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72793486?host=hh.ru </t>
         </is>
       </c>
+      <c r="C399" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="400">
       <c r="A400" t="inlineStr">
@@ -5220,6 +6417,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71060230?host=hh.ru </t>
         </is>
       </c>
+      <c r="C400" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="401">
       <c r="A401" t="inlineStr">
@@ -5232,6 +6432,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71868560?host=hh.ru </t>
         </is>
       </c>
+      <c r="C401" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="402">
       <c r="A402" t="inlineStr">
@@ -5244,6 +6447,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860502?host=hh.ru </t>
         </is>
       </c>
+      <c r="C402" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="403">
       <c r="A403" t="inlineStr">
@@ -5256,6 +6462,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72462248?host=hh.ru </t>
         </is>
       </c>
+      <c r="C403" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="404">
       <c r="A404" t="inlineStr">
@@ -5268,6 +6477,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71660788?host=hh.ru </t>
         </is>
       </c>
+      <c r="C404" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="405">
       <c r="A405" t="inlineStr">
@@ -5280,6 +6492,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72064594?host=hh.ru </t>
         </is>
       </c>
+      <c r="C405" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="406">
       <c r="A406" t="inlineStr">
@@ -5292,6 +6507,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/69870648?host=hh.ru </t>
         </is>
       </c>
+      <c r="C406" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="407">
       <c r="A407" t="inlineStr">
@@ -5304,6 +6522,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71867868?host=hh.ru </t>
         </is>
       </c>
+      <c r="C407" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="408">
       <c r="A408" t="inlineStr">
@@ -5316,6 +6537,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860545?host=hh.ru </t>
         </is>
       </c>
+      <c r="C408" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="409">
       <c r="A409" t="inlineStr">
@@ -5328,6 +6552,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72793855?host=hh.ru </t>
         </is>
       </c>
+      <c r="C409" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="410">
       <c r="A410" t="inlineStr">
@@ -5340,6 +6567,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72793485?host=hh.ru </t>
         </is>
       </c>
+      <c r="C410" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="411">
       <c r="A411" t="inlineStr">
@@ -5352,6 +6582,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860241?host=hh.ru </t>
         </is>
       </c>
+      <c r="C411" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="412">
       <c r="A412" t="inlineStr">
@@ -5364,6 +6597,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72215811?host=hh.ru </t>
         </is>
       </c>
+      <c r="C412" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="413">
       <c r="A413" t="inlineStr">
@@ -5376,6 +6612,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72215748?host=hh.ru </t>
         </is>
       </c>
+      <c r="C413" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="414">
       <c r="A414" t="inlineStr">
@@ -5388,6 +6627,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72215875?host=hh.ru </t>
         </is>
       </c>
+      <c r="C414" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="415">
       <c r="A415" t="inlineStr">
@@ -5400,6 +6642,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71662448?host=hh.ru </t>
         </is>
       </c>
+      <c r="C415" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="416">
       <c r="A416" t="inlineStr">
@@ -5412,6 +6657,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72792956?host=hh.ru </t>
         </is>
       </c>
+      <c r="C416" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="417">
       <c r="A417" t="inlineStr">
@@ -5424,6 +6672,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71911612?host=hh.ru </t>
         </is>
       </c>
+      <c r="C417" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="418">
       <c r="A418" t="inlineStr">
@@ -5436,6 +6687,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/68918046?host=hh.ru </t>
         </is>
       </c>
+      <c r="C418" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="419">
       <c r="A419" t="inlineStr">
@@ -5448,6 +6702,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72215585?host=hh.ru </t>
         </is>
       </c>
+      <c r="C419" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="420">
       <c r="A420" t="inlineStr">
@@ -5460,6 +6717,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66859966?host=hh.ru </t>
         </is>
       </c>
+      <c r="C420" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="421">
       <c r="A421" t="inlineStr">
@@ -5472,6 +6732,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71869516?host=hh.ru </t>
         </is>
       </c>
+      <c r="C421" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="422">
       <c r="A422" t="inlineStr">
@@ -5484,6 +6747,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/70116629?host=hh.ru </t>
         </is>
       </c>
+      <c r="C422" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="423">
       <c r="A423" t="inlineStr">
@@ -5496,6 +6762,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66860045?host=hh.ru </t>
         </is>
       </c>
+      <c r="C423" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="424">
       <c r="A424" t="inlineStr">
@@ -5508,6 +6777,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71661522?host=hh.ru </t>
         </is>
       </c>
+      <c r="C424" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="425">
       <c r="A425" t="inlineStr">
@@ -5520,6 +6792,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71039138?host=hh.ru </t>
         </is>
       </c>
+      <c r="C425" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="426">
       <c r="A426" t="inlineStr">
@@ -5532,6 +6807,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/54368399?host=hh.ru </t>
         </is>
       </c>
+      <c r="C426" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="427">
       <c r="A427" t="inlineStr">
@@ -5544,6 +6822,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72462194?host=hh.ru </t>
         </is>
       </c>
+      <c r="C427" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="428">
       <c r="A428" t="inlineStr">
@@ -5556,6 +6837,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66859874?host=hh.ru </t>
         </is>
       </c>
+      <c r="C428" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="429">
       <c r="A429" t="inlineStr">
@@ -5568,6 +6852,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/66859897?host=hh.ru </t>
         </is>
       </c>
+      <c r="C429" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="430">
       <c r="A430" t="inlineStr">
@@ -5580,6 +6867,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72234058?host=hh.ru </t>
         </is>
       </c>
+      <c r="C430" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="431">
       <c r="A431" t="inlineStr">
@@ -5592,6 +6882,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71883592?host=hh.ru </t>
         </is>
       </c>
+      <c r="C431" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="432">
       <c r="A432" t="inlineStr">
@@ -5604,6 +6897,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71885599?host=hh.ru </t>
         </is>
       </c>
+      <c r="C432" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="433">
       <c r="A433" t="inlineStr">
@@ -5616,6 +6912,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71492524?host=hh.ru </t>
         </is>
       </c>
+      <c r="C433" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="434">
       <c r="A434" t="inlineStr">
@@ -5628,6 +6927,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72793991?host=hh.ru </t>
         </is>
       </c>
+      <c r="C434" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="435">
       <c r="A435" t="inlineStr">
@@ -5640,6 +6942,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71870192?host=hh.ru </t>
         </is>
       </c>
+      <c r="C435" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="436">
       <c r="A436" t="inlineStr">
@@ -5652,6 +6957,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71965320?host=hh.ru </t>
         </is>
       </c>
+      <c r="C436" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="437">
       <c r="A437" t="inlineStr">
@@ -5664,6 +6972,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/71965314?host=hh.ru </t>
         </is>
       </c>
+      <c r="C437" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="438">
       <c r="A438" t="inlineStr">
@@ -5676,6 +6987,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/51251928?host=hh.ru </t>
         </is>
       </c>
+      <c r="C438" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="439">
       <c r="A439" t="inlineStr">
@@ -5688,6 +7002,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/72786037?host=hh.ru </t>
         </is>
       </c>
+      <c r="C439" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="440">
       <c r="A440" t="inlineStr">
@@ -5700,6 +7017,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/68431025?host=hh.ru </t>
         </is>
       </c>
+      <c r="C440" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="441">
       <c r="A441" t="inlineStr">
@@ -5712,6 +7032,9 @@
           <t xml:space="preserve">https://api.hh.ru/vacancies/67876615?host=hh.ru </t>
         </is>
       </c>
+      <c r="C441" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="442">
       <c r="A442" t="inlineStr">
@@ -5723,6 +7046,54 @@
         <is>
           <t xml:space="preserve">https://api.hh.ru/vacancies/72772541?host=hh.ru </t>
         </is>
+      </c>
+      <c r="C442" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>72801067</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://api.hh.ru/vacancies/72801067?host=hh.ru </t>
+        </is>
+      </c>
+      <c r="C443" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>72798766</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://api.hh.ru/vacancies/72798766?host=hh.ru </t>
+        </is>
+      </c>
+      <c r="C444" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>72784352</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://api.hh.ru/vacancies/72784352?host=hh.ru </t>
+        </is>
+      </c>
+      <c r="C445" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>